<commit_message>
Update E11 HR Data - Dashboard.xlsx
</commit_message>
<xml_diff>
--- a/Exercise Files/Exercise 11/E11 HR Data - Dashboard.xlsx
+++ b/Exercise Files/Exercise 11/E11 HR Data - Dashboard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f21e54c367d3358c/Documents/01 Work Files/05 SSIT/Online Courses/Advanced PivotTables/Exercise Files/Exercise 11/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wayvy Technologies\Documents\GitHub\PivotTables\Exercise Files\Exercise 11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="478" documentId="8_{14B10394-980E-4015-BB4E-D9BEE2E7D547}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C2998E9C-E9F7-4893-8ACB-32534505BC65}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB6BA88-1D69-48E3-8A83-086A1669AA75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{960E11C6-F8C0-4296-BE1C-66F0D68FFF3E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="5" xr2:uid="{960E11C6-F8C0-4296-BE1C-66F0D68FFF3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Employee Info" sheetId="1" r:id="rId1"/>
@@ -22,22 +22,23 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Employee Info'!$A$1:$C$100</definedName>
     <definedName name="_xlcn.WorksheetConnection_HRDataConsolidating.xlsxTable11" hidden="1">'Employee Info'!$A$1:$C$100</definedName>
     <definedName name="_xlcn.WorksheetConnection_HRDataConsolidating.xlsxTable21" hidden="1">'[1]Department Info'!$A$1:$A$100</definedName>
-    <definedName name="_xlcn.WorksheetConnection_HRDataConsolidating.xlsxTable31" hidden="1">'[1]Job Info'!$A$1:$A$100</definedName>
+    <definedName name="_xlcn.WorksheetConnection_HRDataConsolidating.xlsxTable31" hidden="1">'[2]Job Info'!$A$1:$A$100</definedName>
     <definedName name="Slicer_Years">#N/A</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="13" r:id="rId8"/>
+    <pivotCache cacheId="0" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
       <x14:slicerCaches>
-        <x14:slicerCache r:id="rId9"/>
+        <x14:slicerCache r:id="rId10"/>
       </x14:slicerCaches>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -113,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="153">
   <si>
     <t>Employee ID</t>
   </si>
@@ -496,9 +497,6 @@
     <t>Grand Total</t>
   </si>
   <si>
-    <t>(All)</t>
-  </si>
-  <si>
     <t>Job Rating</t>
   </si>
   <si>
@@ -514,22 +512,13 @@
     <t>2000</t>
   </si>
   <si>
-    <t>2001</t>
-  </si>
-  <si>
     <t>2002</t>
   </si>
   <si>
     <t>2003</t>
   </si>
   <si>
-    <t>2004</t>
-  </si>
-  <si>
     <t>2005</t>
-  </si>
-  <si>
-    <t>2006</t>
   </si>
   <si>
     <t>2007</t>
@@ -545,9 +534,6 @@
   </si>
   <si>
     <t>2011</t>
-  </si>
-  <si>
-    <t>2012</t>
   </si>
   <si>
     <t>2013</t>
@@ -655,7 +641,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -663,7 +649,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1776,6 +1761,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1073975535"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1835,6 +1821,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1446685311"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
@@ -9092,8 +9079,8 @@
       <xdr:row>22</xdr:row>
       <xdr:rowOff>15241</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="12" name="Years">
@@ -9116,7 +9103,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -9267,15 +9254,26 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Department Info"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
       <sheetName val="Job Info"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -10708,7 +10706,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9A9DE2D2-A8AE-433E-9905-5FCD4B93F589}" name="PivotTable3" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9A9DE2D2-A8AE-433E-9905-5FCD4B93F589}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A3:B6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -10894,7 +10892,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2E992F78-E056-4116-B9D9-9D8F1A2F3FEB}" name="PivotTable3" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2E992F78-E056-4116-B9D9-9D8F1A2F3FEB}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A3:B6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -11070,7 +11068,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CFFE7B5C-571C-42D2-8AD9-3215FA5C6911}" name="PivotTable3" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" showDrill="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CFFE7B5C-571C-42D2-8AD9-3215FA5C6911}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" showDrill="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -11326,8 +11324,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D43F3D8F-85B4-4648-9F8E-FD882E6CABCC}" name="PivotTable3" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" showDrill="0" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
-  <location ref="A3:H25" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D43F3D8F-85B4-4648-9F8E-FD882E6CABCC}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="8" minRefreshableVersion="3" showDrill="0" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
+  <location ref="A3:G21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
     <pivotField showAll="0">
@@ -11466,10 +11464,10 @@
       </items>
     </pivotField>
     <pivotField dataField="1" numFmtId="44" showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
       <items count="3">
         <item x="1"/>
-        <item x="0"/>
+        <item h="1" x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -11536,12 +11534,9 @@
   <rowFields count="1">
     <field x="10"/>
   </rowFields>
-  <rowItems count="21">
+  <rowItems count="17">
     <i>
       <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
     </i>
     <i>
       <x v="3"/>
@@ -11550,13 +11545,7 @@
       <x v="4"/>
     </i>
     <i>
-      <x v="5"/>
-    </i>
-    <i>
       <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
     </i>
     <i>
       <x v="8"/>
@@ -11572,9 +11561,6 @@
     </i>
     <i>
       <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
     </i>
     <i>
       <x v="14"/>
@@ -11604,7 +11590,7 @@
   <colFields count="1">
     <field x="3"/>
   </colFields>
-  <colItems count="7">
+  <colItems count="6">
     <i>
       <x/>
     </i>
@@ -11622,9 +11608,6 @@
     </i>
     <i>
       <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
     </i>
   </colItems>
   <pageFields count="1">
@@ -11707,9 +11690,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -11747,7 +11730,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -11853,7 +11836,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -11995,7 +11978,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -12009,19 +11992,19 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="22.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" customWidth="1"/>
-    <col min="6" max="6" width="24.109375" style="1" customWidth="1"/>
-    <col min="7" max="8" width="20.21875" customWidth="1"/>
-    <col min="9" max="9" width="18.21875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="20.28515625" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -12044,13 +12027,13 @@
         <v>121</v>
       </c>
       <c r="H1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2100</v>
       </c>
@@ -12079,7 +12062,7 @@
         <v>40445</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2101</v>
       </c>
@@ -12108,7 +12091,7 @@
         <v>42551</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2102</v>
       </c>
@@ -12137,7 +12120,7 @@
         <v>43376</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2103</v>
       </c>
@@ -12166,7 +12149,7 @@
         <v>43168</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2104</v>
       </c>
@@ -12195,7 +12178,7 @@
         <v>40164</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2105</v>
       </c>
@@ -12224,7 +12207,7 @@
         <v>40511</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2106</v>
       </c>
@@ -12253,7 +12236,7 @@
         <v>43915</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2107</v>
       </c>
@@ -12282,7 +12265,7 @@
         <v>38555</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2108</v>
       </c>
@@ -12311,7 +12294,7 @@
         <v>42421</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2109</v>
       </c>
@@ -12340,7 +12323,7 @@
         <v>43151</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2110</v>
       </c>
@@ -12369,7 +12352,7 @@
         <v>42809</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2111</v>
       </c>
@@ -12398,7 +12381,7 @@
         <v>40378</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2112</v>
       </c>
@@ -12427,7 +12410,7 @@
         <v>40976</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2113</v>
       </c>
@@ -12456,7 +12439,7 @@
         <v>36845</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2114</v>
       </c>
@@ -12485,7 +12468,7 @@
         <v>42217</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2115</v>
       </c>
@@ -12514,7 +12497,7 @@
         <v>41198</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2116</v>
       </c>
@@ -12543,7 +12526,7 @@
         <v>36704</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2117</v>
       </c>
@@ -12572,7 +12555,7 @@
         <v>42895</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2118</v>
       </c>
@@ -12601,7 +12584,7 @@
         <v>41286</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2119</v>
       </c>
@@ -12630,7 +12613,7 @@
         <v>39319</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2120</v>
       </c>
@@ -12659,7 +12642,7 @@
         <v>40839</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2121</v>
       </c>
@@ -12688,7 +12671,7 @@
         <v>36754</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2122</v>
       </c>
@@ -12717,7 +12700,7 @@
         <v>38170</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2123</v>
       </c>
@@ -12746,7 +12729,7 @@
         <v>39164</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2124</v>
       </c>
@@ -12775,7 +12758,7 @@
         <v>42219</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2125</v>
       </c>
@@ -12804,7 +12787,7 @@
         <v>40652</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2126</v>
       </c>
@@ -12833,7 +12816,7 @@
         <v>41065</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2127</v>
       </c>
@@ -12862,7 +12845,7 @@
         <v>39692</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2128</v>
       </c>
@@ -12891,7 +12874,7 @@
         <v>42030</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2129</v>
       </c>
@@ -12920,7 +12903,7 @@
         <v>39499</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2130</v>
       </c>
@@ -12949,7 +12932,7 @@
         <v>43695</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2131</v>
       </c>
@@ -12978,7 +12961,7 @@
         <v>42324</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2132</v>
       </c>
@@ -13007,7 +12990,7 @@
         <v>36600</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2133</v>
       </c>
@@ -13036,7 +13019,7 @@
         <v>39803</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2134</v>
       </c>
@@ -13065,7 +13048,7 @@
         <v>40249</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2135</v>
       </c>
@@ -13094,7 +13077,7 @@
         <v>38971</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2136</v>
       </c>
@@ -13123,7 +13106,7 @@
         <v>40276</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2137</v>
       </c>
@@ -13152,7 +13135,7 @@
         <v>38241</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2138</v>
       </c>
@@ -13181,7 +13164,7 @@
         <v>40684</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2139</v>
       </c>
@@ -13210,7 +13193,7 @@
         <v>39996</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2140</v>
       </c>
@@ -13239,7 +13222,7 @@
         <v>37411</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2141</v>
       </c>
@@ -13268,7 +13251,7 @@
         <v>43850</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2142</v>
       </c>
@@ -13297,7 +13280,7 @@
         <v>43170</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2143</v>
       </c>
@@ -13326,7 +13309,7 @@
         <v>37292</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2144</v>
       </c>
@@ -13355,7 +13338,7 @@
         <v>37609</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2145</v>
       </c>
@@ -13384,7 +13367,7 @@
         <v>37094</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2146</v>
       </c>
@@ -13413,7 +13396,7 @@
         <v>42118</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2147</v>
       </c>
@@ -13442,7 +13425,7 @@
         <v>41517</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2148</v>
       </c>
@@ -13471,7 +13454,7 @@
         <v>38742</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2149</v>
       </c>
@@ -13500,7 +13483,7 @@
         <v>40047</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2150</v>
       </c>
@@ -13529,7 +13512,7 @@
         <v>39802</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2151</v>
       </c>
@@ -13558,7 +13541,7 @@
         <v>39616</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2152</v>
       </c>
@@ -13587,7 +13570,7 @@
         <v>41686</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2153</v>
       </c>
@@ -13616,7 +13599,7 @@
         <v>39019</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2154</v>
       </c>
@@ -13645,7 +13628,7 @@
         <v>41028</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2155</v>
       </c>
@@ -13674,7 +13657,7 @@
         <v>39768</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2156</v>
       </c>
@@ -13703,7 +13686,7 @@
         <v>41153</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2157</v>
       </c>
@@ -13732,7 +13715,7 @@
         <v>36847</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2158</v>
       </c>
@@ -13761,7 +13744,7 @@
         <v>37105</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2159</v>
       </c>
@@ -13790,7 +13773,7 @@
         <v>39744</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2160</v>
       </c>
@@ -13819,7 +13802,7 @@
         <v>43167</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2161</v>
       </c>
@@ -13848,7 +13831,7 @@
         <v>38401</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2162</v>
       </c>
@@ -13877,7 +13860,7 @@
         <v>37956</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2163</v>
       </c>
@@ -13906,7 +13889,7 @@
         <v>43907</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2164</v>
       </c>
@@ -13935,7 +13918,7 @@
         <v>43669</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2165</v>
       </c>
@@ -13964,7 +13947,7 @@
         <v>39740</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2166</v>
       </c>
@@ -13993,7 +13976,7 @@
         <v>40408</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2167</v>
       </c>
@@ -14022,7 +14005,7 @@
         <v>38822</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2168</v>
       </c>
@@ -14051,7 +14034,7 @@
         <v>40083</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2169</v>
       </c>
@@ -14080,7 +14063,7 @@
         <v>41579</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2170</v>
       </c>
@@ -14109,7 +14092,7 @@
         <v>43027</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2171</v>
       </c>
@@ -14138,7 +14121,7 @@
         <v>41582</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2172</v>
       </c>
@@ -14167,7 +14150,7 @@
         <v>36663</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2173</v>
       </c>
@@ -14196,7 +14179,7 @@
         <v>37526</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2174</v>
       </c>
@@ -14225,7 +14208,7 @@
         <v>41710</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2175</v>
       </c>
@@ -14254,7 +14237,7 @@
         <v>40274</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2176</v>
       </c>
@@ -14283,7 +14266,7 @@
         <v>40107</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2177</v>
       </c>
@@ -14312,7 +14295,7 @@
         <v>39142</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2178</v>
       </c>
@@ -14341,7 +14324,7 @@
         <v>39165</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2179</v>
       </c>
@@ -14370,7 +14353,7 @@
         <v>42462</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2180</v>
       </c>
@@ -14399,7 +14382,7 @@
         <v>41654</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>2181</v>
       </c>
@@ -14428,7 +14411,7 @@
         <v>43128</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2182</v>
       </c>
@@ -14457,7 +14440,7 @@
         <v>43381</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>2183</v>
       </c>
@@ -14486,7 +14469,7 @@
         <v>41676</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2184</v>
       </c>
@@ -14515,7 +14498,7 @@
         <v>36651</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>2185</v>
       </c>
@@ -14544,7 +14527,7 @@
         <v>42526</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2186</v>
       </c>
@@ -14573,7 +14556,7 @@
         <v>38565</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2187</v>
       </c>
@@ -14602,7 +14585,7 @@
         <v>37518</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>2188</v>
       </c>
@@ -14631,7 +14614,7 @@
         <v>39656</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>2189</v>
       </c>
@@ -14660,7 +14643,7 @@
         <v>41701</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>2190</v>
       </c>
@@ -14689,7 +14672,7 @@
         <v>42528</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>2191</v>
       </c>
@@ -14718,7 +14701,7 @@
         <v>38499</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>2192</v>
       </c>
@@ -14747,7 +14730,7 @@
         <v>43550</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>2193</v>
       </c>
@@ -14776,7 +14759,7 @@
         <v>38384</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>2194</v>
       </c>
@@ -14805,7 +14788,7 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>2195</v>
       </c>
@@ -14834,7 +14817,7 @@
         <v>43124</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>2196</v>
       </c>
@@ -14863,7 +14846,7 @@
         <v>37442</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2197</v>
       </c>
@@ -14892,7 +14875,7 @@
         <v>38690</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>2198</v>
       </c>
@@ -14937,41 +14920,41 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>125</v>
       </c>
       <c r="B3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>0.6262626262626263</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="7">
         <v>0.37373737373737376</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="7">
         <v>1</v>
       </c>
     </row>
@@ -14989,41 +14972,41 @@
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>125</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>64650.741935483871</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>62631.891891891893</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>63896.222222222219</v>
       </c>
     </row>
@@ -15041,73 +15024,73 @@
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>125</v>
       </c>
       <c r="B3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="B4" s="5">
-        <v>5</v>
+      <c r="B9">
+        <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="B5" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="B6" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="B7" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="B8" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="B9" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10">
         <v>28</v>
       </c>
     </row>
@@ -15119,133 +15102,132 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E674423-ACA0-4EAC-BB7D-3943C7AB7B54}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="10" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="14" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="10" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="61" max="61" width="10" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="63" max="64" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="83" max="83" width="16" bestFit="1" customWidth="1"/>
     <col min="84" max="84" width="12" bestFit="1" customWidth="1"/>
     <col min="85" max="85" width="11" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="91" max="91" width="14" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="94" max="94" width="11" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="98" max="98" width="14" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>121</v>
       </c>
       <c r="B1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>125</v>
       </c>
@@ -15267,553 +15249,395 @@
       <c r="G4" t="s">
         <v>107</v>
       </c>
-      <c r="H4" t="s">
-        <v>110</v>
-      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" s="5">
+        <v>99568</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5">
+        <v>72568</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5">
+        <v>78859</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="B5" s="6">
-        <v>99568</v>
-      </c>
-      <c r="C5" s="6">
-        <v>33778</v>
-      </c>
-      <c r="D5" s="6">
-        <v>72568</v>
-      </c>
-      <c r="E5" s="6">
+      <c r="B6" s="5">
         <v>0</v>
       </c>
-      <c r="F5" s="6">
-        <v>32929</v>
-      </c>
-      <c r="G5" s="6">
-        <v>217879</v>
-      </c>
-      <c r="H5" s="6">
+      <c r="C6" s="5">
         <v>0</v>
       </c>
+      <c r="D6" s="5">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5">
+        <v>47939</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B7" s="5">
         <v>0</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C7" s="5">
         <v>0</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D7" s="5">
         <v>0</v>
       </c>
-      <c r="E6" s="6">
-        <v>45587</v>
-      </c>
-      <c r="F6" s="6">
+      <c r="E7" s="5">
         <v>0</v>
       </c>
-      <c r="G6" s="6">
-        <v>83237</v>
-      </c>
-      <c r="H6" s="6">
+      <c r="F7" s="5">
+        <v>62472</v>
+      </c>
+      <c r="G7" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="B7" s="6">
-        <v>38206</v>
-      </c>
-      <c r="C7" s="6">
-        <v>47199</v>
-      </c>
-      <c r="D7" s="6">
-        <v>40979</v>
-      </c>
-      <c r="E7" s="6">
-        <v>91632</v>
-      </c>
-      <c r="F7" s="6">
+      <c r="B8" s="5">
         <v>0</v>
       </c>
-      <c r="G7" s="6">
-        <v>47939</v>
-      </c>
-      <c r="H7" s="6">
-        <v>59404</v>
+      <c r="C8" s="5">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0</v>
+      </c>
+      <c r="G8" s="5">
+        <v>37471</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B9" s="5">
         <v>0</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C9" s="5">
+        <v>56445</v>
+      </c>
+      <c r="D9" s="5">
         <v>0</v>
       </c>
-      <c r="D8" s="6">
+      <c r="E9" s="5">
         <v>0</v>
       </c>
-      <c r="E8" s="6">
+      <c r="F9" s="5">
         <v>0</v>
       </c>
-      <c r="F8" s="6">
-        <v>62472</v>
-      </c>
-      <c r="G8" s="6">
+      <c r="G9" s="5">
         <v>0</v>
       </c>
-      <c r="H8" s="6">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B10" s="5">
         <v>0</v>
       </c>
+      <c r="C10" s="5">
+        <v>70918</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="B9" s="6">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B11" s="5">
+        <v>48094</v>
+      </c>
+      <c r="C11" s="5">
         <v>0</v>
       </c>
-      <c r="C9" s="6">
-        <v>56146</v>
-      </c>
-      <c r="D9" s="6">
+      <c r="D11" s="5">
         <v>0</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E11" s="5">
         <v>0</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F11" s="5">
+        <v>25504</v>
+      </c>
+      <c r="G11" s="5">
         <v>0</v>
       </c>
-      <c r="G9" s="6">
-        <v>74903</v>
-      </c>
-      <c r="H9" s="6">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B12" s="5">
         <v>0</v>
       </c>
+      <c r="C12" s="5">
+        <v>83169</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="B10" s="6">
-        <v>111139</v>
-      </c>
-      <c r="C10" s="6">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B13" s="5">
         <v>0</v>
       </c>
-      <c r="D10" s="6">
-        <v>33900</v>
-      </c>
-      <c r="E10" s="6">
+      <c r="C13" s="5">
         <v>0</v>
       </c>
-      <c r="F10" s="6">
+      <c r="D13" s="5">
         <v>0</v>
       </c>
-      <c r="G10" s="6">
-        <v>127799</v>
-      </c>
-      <c r="H10" s="6">
-        <v>85414</v>
+      <c r="E13" s="5">
+        <v>74201</v>
+      </c>
+      <c r="F13" s="5">
+        <v>74344</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="B11" s="6">
-        <v>61955</v>
-      </c>
-      <c r="C11" s="6">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B14" s="5">
         <v>0</v>
       </c>
-      <c r="D11" s="6">
-        <v>164120</v>
-      </c>
-      <c r="E11" s="6">
+      <c r="C14" s="5">
         <v>0</v>
       </c>
-      <c r="F11" s="6">
-        <v>50441</v>
-      </c>
-      <c r="G11" s="6">
+      <c r="D14" s="5">
+        <v>47852</v>
+      </c>
+      <c r="E14" s="5">
         <v>0</v>
       </c>
-      <c r="H11" s="6">
+      <c r="F14" s="5">
         <v>0</v>
       </c>
+      <c r="G14" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B12" s="6">
-        <v>78844</v>
-      </c>
-      <c r="C12" s="6">
-        <v>56445</v>
-      </c>
-      <c r="D12" s="6">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B15" s="5">
         <v>0</v>
       </c>
-      <c r="E12" s="6">
+      <c r="C15" s="5">
         <v>0</v>
       </c>
-      <c r="F12" s="6">
+      <c r="D15" s="5">
         <v>0</v>
       </c>
-      <c r="G12" s="6">
-        <v>89126</v>
-      </c>
-      <c r="H12" s="6">
-        <v>67560</v>
+      <c r="E15" s="5">
+        <v>96503</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0</v>
+      </c>
+      <c r="G15" s="5">
+        <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="B13" s="6">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B16" s="5">
+        <v>156781</v>
+      </c>
+      <c r="C16" s="5">
         <v>0</v>
       </c>
-      <c r="C13" s="6">
-        <v>134580</v>
-      </c>
-      <c r="D13" s="6">
-        <v>165268</v>
-      </c>
-      <c r="E13" s="6">
-        <v>61939</v>
-      </c>
-      <c r="F13" s="6">
-        <v>86778</v>
-      </c>
-      <c r="G13" s="6">
-        <v>89358</v>
-      </c>
-      <c r="H13" s="6">
-        <v>29892</v>
+      <c r="D16" s="5">
+        <v>97719</v>
+      </c>
+      <c r="E16" s="5">
+        <v>87541</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0</v>
+      </c>
+      <c r="G16" s="5">
+        <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="B14" s="6">
-        <v>135471</v>
-      </c>
-      <c r="C14" s="6">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B17" s="5">
         <v>0</v>
       </c>
-      <c r="D14" s="6">
-        <v>145008</v>
-      </c>
-      <c r="E14" s="6">
+      <c r="C17" s="5">
         <v>0</v>
       </c>
-      <c r="F14" s="6">
-        <v>25504</v>
-      </c>
-      <c r="G14" s="6">
+      <c r="D17" s="5">
         <v>0</v>
       </c>
-      <c r="H14" s="6">
+      <c r="E17" s="5">
         <v>0</v>
       </c>
+      <c r="F17" s="5">
+        <v>33787</v>
+      </c>
+      <c r="G17" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="B15" s="6">
-        <v>162347</v>
-      </c>
-      <c r="C15" s="6">
-        <v>83169</v>
-      </c>
-      <c r="D15" s="6">
-        <v>26402</v>
-      </c>
-      <c r="E15" s="6">
-        <v>51225</v>
-      </c>
-      <c r="F15" s="6">
-        <v>90608</v>
-      </c>
-      <c r="G15" s="6">
-        <v>60066</v>
-      </c>
-      <c r="H15" s="6">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B18" s="5">
+        <v>71067</v>
+      </c>
+      <c r="C18" s="5">
         <v>0</v>
       </c>
+      <c r="D18" s="5">
+        <v>0</v>
+      </c>
+      <c r="E18" s="5">
+        <v>84304</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0</v>
+      </c>
+      <c r="G18" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="B16" s="6">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B19" s="5">
+        <v>86734</v>
+      </c>
+      <c r="C19" s="5">
         <v>0</v>
       </c>
-      <c r="C16" s="6">
+      <c r="D19" s="5">
+        <v>55197</v>
+      </c>
+      <c r="E19" s="5">
         <v>0</v>
       </c>
-      <c r="D16" s="6">
-        <v>55175</v>
-      </c>
-      <c r="E16" s="6">
-        <v>74201</v>
-      </c>
-      <c r="F16" s="6">
-        <v>74344</v>
-      </c>
-      <c r="G16" s="6">
+      <c r="F19" s="5">
         <v>0</v>
       </c>
-      <c r="H16" s="6">
+      <c r="G19" s="5">
+        <v>39748</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B20" s="5">
         <v>0</v>
       </c>
+      <c r="C20" s="5">
+        <v>86357</v>
+      </c>
+      <c r="D20" s="5">
+        <v>0</v>
+      </c>
+      <c r="E20" s="5">
+        <v>0</v>
+      </c>
+      <c r="F20" s="5">
+        <v>0</v>
+      </c>
+      <c r="G20" s="5">
+        <v>43304</v>
+      </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="B17" s="6">
-        <v>79270</v>
-      </c>
-      <c r="C17" s="6">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B21" s="5">
         <v>0</v>
       </c>
-      <c r="D17" s="6">
+      <c r="C21" s="5">
         <v>0</v>
       </c>
-      <c r="E17" s="6">
+      <c r="D21" s="5">
         <v>0</v>
       </c>
-      <c r="F17" s="6">
+      <c r="E21" s="5">
         <v>0</v>
       </c>
-      <c r="G17" s="6">
-        <v>56934</v>
-      </c>
-      <c r="H17" s="6">
-        <v>257158</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="B18" s="6">
-        <v>50831</v>
-      </c>
-      <c r="C18" s="6">
-        <v>57759</v>
-      </c>
-      <c r="D18" s="6">
-        <v>47852</v>
-      </c>
-      <c r="E18" s="6">
-        <v>0</v>
-      </c>
-      <c r="F18" s="6">
-        <v>0</v>
-      </c>
-      <c r="G18" s="6">
-        <v>0</v>
-      </c>
-      <c r="H18" s="6">
-        <v>62997</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="B19" s="6">
-        <v>0</v>
-      </c>
-      <c r="C19" s="6">
-        <v>0</v>
-      </c>
-      <c r="D19" s="6">
-        <v>84859</v>
-      </c>
-      <c r="E19" s="6">
-        <v>189029</v>
-      </c>
-      <c r="F19" s="6">
-        <v>82871</v>
-      </c>
-      <c r="G19" s="6">
-        <v>0</v>
-      </c>
-      <c r="H19" s="6">
-        <v>91367</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="B20" s="6">
-        <v>156781</v>
-      </c>
-      <c r="C20" s="6">
-        <v>0</v>
-      </c>
-      <c r="D20" s="6">
-        <v>97719</v>
-      </c>
-      <c r="E20" s="6">
-        <v>115255</v>
-      </c>
-      <c r="F20" s="6">
-        <v>0</v>
-      </c>
-      <c r="G20" s="6">
-        <v>0</v>
-      </c>
-      <c r="H20" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="B21" s="6">
-        <v>0</v>
-      </c>
-      <c r="C21" s="6">
-        <v>74324</v>
-      </c>
-      <c r="D21" s="6">
-        <v>0</v>
-      </c>
-      <c r="E21" s="6">
-        <v>95346</v>
-      </c>
-      <c r="F21" s="6">
-        <v>33787</v>
-      </c>
-      <c r="G21" s="6">
-        <v>109740</v>
-      </c>
-      <c r="H21" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="B22" s="6">
-        <v>71067</v>
-      </c>
-      <c r="C22" s="6">
-        <v>0</v>
-      </c>
-      <c r="D22" s="6">
-        <v>0</v>
-      </c>
-      <c r="E22" s="6">
-        <v>138406</v>
-      </c>
-      <c r="F22" s="6">
-        <v>0</v>
-      </c>
-      <c r="G22" s="6">
-        <v>0</v>
-      </c>
-      <c r="H22" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="B23" s="6">
-        <v>180784</v>
-      </c>
-      <c r="C23" s="6">
-        <v>0</v>
-      </c>
-      <c r="D23" s="6">
-        <v>145936</v>
-      </c>
-      <c r="E23" s="6">
-        <v>40689</v>
-      </c>
-      <c r="F23" s="6">
-        <v>0</v>
-      </c>
-      <c r="G23" s="6">
-        <v>66825</v>
-      </c>
-      <c r="H23" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="B24" s="6">
-        <v>0</v>
-      </c>
-      <c r="C24" s="6">
-        <v>156442</v>
-      </c>
-      <c r="D24" s="6">
-        <v>0</v>
-      </c>
-      <c r="E24" s="6">
-        <v>0</v>
-      </c>
-      <c r="F24" s="6">
-        <v>0</v>
-      </c>
-      <c r="G24" s="6">
-        <v>43304</v>
-      </c>
-      <c r="H24" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="B25" s="6">
-        <v>32172</v>
-      </c>
-      <c r="C25" s="6">
-        <v>0</v>
-      </c>
-      <c r="D25" s="6">
-        <v>0</v>
-      </c>
-      <c r="E25" s="6">
-        <v>0</v>
-      </c>
-      <c r="F25" s="6">
-        <v>123718</v>
-      </c>
-      <c r="G25" s="6">
-        <v>0</v>
-      </c>
-      <c r="H25" s="6">
+      <c r="F21" s="5">
+        <v>52320</v>
+      </c>
+      <c r="G21" s="5">
         <v>0</v>
       </c>
     </row>
@@ -15826,162 +15650,162 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADA24C5-9622-4DB4-B0A6-9CD405FC464F}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="3.44140625" customWidth="1"/>
+    <col min="4" max="4" width="3.42578125" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" customWidth="1"/>
-    <col min="8" max="8" width="13.88671875" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="9" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>156</v>
+    <row r="1" spans="1:1" s="8" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>151</v>
       </c>
     </row>
-    <row r="24" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E24" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="G24" s="10" t="s">
+    <row r="24" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E24" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="G24" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="H24" s="10" t="s">
-        <v>155</v>
+      <c r="H24" s="9" t="s">
+        <v>150</v>
       </c>
     </row>
-    <row r="25" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E25" s="7" t="str">
+    <row r="25" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E25" s="6" t="str">
         <f>Sparklines!A5</f>
         <v>2000</v>
       </c>
     </row>
-    <row r="26" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E26" s="7" t="str">
+    <row r="26" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E26" s="6" t="str">
         <f>Sparklines!A6</f>
-        <v>2001</v>
+        <v>2002</v>
       </c>
     </row>
-    <row r="27" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E27" s="7" t="str">
+    <row r="27" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E27" s="6" t="str">
         <f>Sparklines!A7</f>
-        <v>2002</v>
+        <v>2003</v>
       </c>
     </row>
-    <row r="28" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E28" s="7" t="str">
+    <row r="28" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E28" s="6" t="str">
         <f>Sparklines!A8</f>
-        <v>2003</v>
+        <v>2005</v>
       </c>
     </row>
-    <row r="29" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E29" s="7" t="str">
+    <row r="29" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E29" s="6" t="str">
         <f>Sparklines!A9</f>
-        <v>2004</v>
+        <v>2007</v>
       </c>
     </row>
-    <row r="30" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E30" s="7" t="str">
+    <row r="30" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E30" s="6" t="str">
         <f>Sparklines!A10</f>
-        <v>2005</v>
+        <v>2008</v>
       </c>
     </row>
-    <row r="31" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E31" s="7" t="str">
+    <row r="31" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E31" s="6" t="str">
         <f>Sparklines!A11</f>
-        <v>2006</v>
+        <v>2009</v>
       </c>
     </row>
-    <row r="32" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E32" s="7" t="str">
+    <row r="32" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E32" s="6" t="str">
         <f>Sparklines!A12</f>
-        <v>2007</v>
+        <v>2010</v>
       </c>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E33" s="7" t="str">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="6" t="str">
         <f>Sparklines!A13</f>
-        <v>2008</v>
+        <v>2011</v>
       </c>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E34" s="7" t="str">
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="6" t="str">
         <f>Sparklines!A14</f>
-        <v>2009</v>
+        <v>2013</v>
       </c>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E35" s="7" t="str">
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="6" t="str">
         <f>Sparklines!A15</f>
-        <v>2010</v>
+        <v>2014</v>
       </c>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E36" s="7" t="str">
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="6" t="str">
         <f>Sparklines!A16</f>
-        <v>2011</v>
+        <v>2015</v>
       </c>
     </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E37" s="7" t="str">
+    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E37" s="6" t="str">
         <f>Sparklines!A17</f>
-        <v>2012</v>
+        <v>2016</v>
       </c>
     </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E38" s="7" t="str">
+    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E38" s="6" t="str">
         <f>Sparklines!A18</f>
-        <v>2013</v>
+        <v>2017</v>
       </c>
     </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E39" s="7" t="str">
+    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E39" s="6" t="str">
         <f>Sparklines!A19</f>
-        <v>2014</v>
+        <v>2018</v>
       </c>
     </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E40" s="7" t="str">
+    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E40" s="6" t="str">
         <f>Sparklines!A20</f>
-        <v>2015</v>
+        <v>2019</v>
       </c>
     </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E41" s="7" t="str">
+    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E41" s="6" t="str">
         <f>Sparklines!A21</f>
-        <v>2016</v>
+        <v>2020</v>
       </c>
     </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E42" s="7" t="str">
+    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E42" s="6">
         <f>Sparklines!A22</f>
-        <v>2017</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E43" s="7" t="str">
+    <row r="43" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E43" s="6">
         <f>Sparklines!A23</f>
-        <v>2018</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="44" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E44" s="7" t="str">
+    <row r="44" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E44" s="6">
         <f>Sparklines!A24</f>
-        <v>2019</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="45" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E45" s="7" t="str">
+    <row r="45" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E45" s="6">
         <f>Sparklines!A25</f>
-        <v>2020</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -15990,6 +15814,178 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{E36CAE45-F631-470C-A7C2-C275262A3DB9}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Sparklines!B5:H5</xm:f>
+              <xm:sqref>H25</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sparklines!B6:H6</xm:f>
+              <xm:sqref>H26</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sparklines!B7:H7</xm:f>
+              <xm:sqref>H27</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sparklines!B8:H8</xm:f>
+              <xm:sqref>H28</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sparklines!B9:H9</xm:f>
+              <xm:sqref>H29</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sparklines!B10:H10</xm:f>
+              <xm:sqref>H30</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sparklines!B11:H11</xm:f>
+              <xm:sqref>H31</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sparklines!B12:H12</xm:f>
+              <xm:sqref>H32</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sparklines!B13:H13</xm:f>
+              <xm:sqref>H33</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sparklines!B14:H14</xm:f>
+              <xm:sqref>H34</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sparklines!B15:H15</xm:f>
+              <xm:sqref>H35</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sparklines!B16:H16</xm:f>
+              <xm:sqref>H36</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sparklines!B17:H17</xm:f>
+              <xm:sqref>H37</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sparklines!B18:H18</xm:f>
+              <xm:sqref>H38</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sparklines!B19:H19</xm:f>
+              <xm:sqref>H39</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sparklines!B20:H20</xm:f>
+              <xm:sqref>H40</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sparklines!B21:H21</xm:f>
+              <xm:sqref>H41</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sparklines!B22:H22</xm:f>
+              <xm:sqref>H42</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sparklines!B23:H23</xm:f>
+              <xm:sqref>H43</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sparklines!B24:H24</xm:f>
+              <xm:sqref>H44</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{5BD8B78E-1297-4339-835F-849347DE66B8}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Sparklines!B5:G5</xm:f>
+              <xm:sqref>G25</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sparklines!B6:G6</xm:f>
+              <xm:sqref>G26</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sparklines!B7:G7</xm:f>
+              <xm:sqref>G27</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sparklines!B8:G8</xm:f>
+              <xm:sqref>G28</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sparklines!B9:G9</xm:f>
+              <xm:sqref>G29</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sparklines!B10:G10</xm:f>
+              <xm:sqref>G30</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sparklines!B11:G11</xm:f>
+              <xm:sqref>G31</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sparklines!B12:G12</xm:f>
+              <xm:sqref>G32</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sparklines!B13:G13</xm:f>
+              <xm:sqref>G33</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sparklines!B14:G14</xm:f>
+              <xm:sqref>G34</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sparklines!B15:G15</xm:f>
+              <xm:sqref>G35</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sparklines!B16:G16</xm:f>
+              <xm:sqref>G36</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sparklines!B17:G17</xm:f>
+              <xm:sqref>G37</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sparklines!B18:G18</xm:f>
+              <xm:sqref>G38</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sparklines!B19:G19</xm:f>
+              <xm:sqref>G39</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sparklines!B20:G20</xm:f>
+              <xm:sqref>G40</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sparklines!B21:G21</xm:f>
+              <xm:sqref>G41</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
         <x14:sparklineGroup displayEmptyCellsAs="gap" high="1" low="1" first="1" last="1" xr2:uid="{FC56BB0D-3489-4CB6-A715-94586F7C5255}">
           <x14:colorSeries theme="4" tint="-0.499984740745262"/>
           <x14:colorNegative theme="5"/>

</xml_diff>